<commit_message>
refactor: folder structure and libs
</commit_message>
<xml_diff>
--- a/enriched_company_data.xlsx
+++ b/enriched_company_data.xlsx
@@ -436,10 +436,10 @@
     <col width="31" customWidth="1" min="1" max="1"/>
     <col width="32" customWidth="1" min="2" max="2"/>
     <col width="55" customWidth="1" min="3" max="3"/>
-    <col width="30" customWidth="1" min="4" max="4"/>
+    <col width="31" customWidth="1" min="4" max="4"/>
     <col width="24" customWidth="1" min="5" max="5"/>
     <col width="15" customWidth="1" min="6" max="6"/>
-    <col width="37" customWidth="1" min="7" max="7"/>
+    <col width="36" customWidth="1" min="7" max="7"/>
     <col width="28" customWidth="1" min="8" max="8"/>
     <col width="64" customWidth="1" min="9" max="9"/>
     <col width="12" customWidth="1" min="10" max="10"/>
@@ -521,7 +521,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Access 1 employee</t>
+          <t>Discover 1 employee</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -550,7 +550,7 @@
         </is>
       </c>
       <c r="J2" t="n">
-        <v>1632100</v>
+        <v>6704018</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
@@ -747,7 +747,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Access all 659 employees</t>
+          <t>View all 659 employees</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -776,7 +776,7 @@
         </is>
       </c>
       <c r="J6" t="n">
-        <v>8478314</v>
+        <v>2273792</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
@@ -916,7 +916,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Access all 3,354 employees</t>
+          <t>Access all 3,353 employees</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -945,7 +945,7 @@
         </is>
       </c>
       <c r="J9" t="n">
-        <v>2819095</v>
+        <v>2444446</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
@@ -1199,7 +1199,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>View all 120 employees</t>
+          <t>Access all 120 employees</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1228,7 +1228,7 @@
         </is>
       </c>
       <c r="J14" t="n">
-        <v>6293113</v>
+        <v>7615115</v>
       </c>
       <c r="K14" t="inlineStr">
         <is>
@@ -1254,7 +1254,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Access all 3,787 employees</t>
+          <t>Discover all 3,795 employees</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1283,7 +1283,7 @@
         </is>
       </c>
       <c r="J15" t="n">
-        <v>7619631</v>
+        <v>1856460</v>
       </c>
       <c r="K15" t="inlineStr">
         <is>
@@ -1309,7 +1309,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Access all 2,043 employees</t>
+          <t>View all 2,043 employees</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1338,7 +1338,7 @@
         </is>
       </c>
       <c r="J16" t="n">
-        <v>6829123</v>
+        <v>5978459</v>
       </c>
       <c r="K16" t="inlineStr">
         <is>
@@ -1592,7 +1592,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>View all 10 employees</t>
+          <t>Discover all 10 employees</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1621,7 +1621,7 @@
         </is>
       </c>
       <c r="J21" t="n">
-        <v>7778768</v>
+        <v>6230607</v>
       </c>
       <c r="K21" t="inlineStr">
         <is>
@@ -1647,7 +1647,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Access all 1,723 employees</t>
+          <t>Discover all 1,723 employees</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1676,7 +1676,7 @@
         </is>
       </c>
       <c r="J22" t="n">
-        <v>6536683</v>
+        <v>9770839</v>
       </c>
       <c r="K22" t="inlineStr">
         <is>
@@ -1759,7 +1759,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Access all 20 employees</t>
+          <t>View all 20 employees</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1788,7 +1788,7 @@
         </is>
       </c>
       <c r="J24" t="n">
-        <v>1893160</v>
+        <v>9766198</v>
       </c>
       <c r="K24" t="inlineStr">
         <is>
@@ -1814,7 +1814,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>View all 27,037 employees</t>
+          <t>Discover all 27,036 employees</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1843,7 +1843,7 @@
         </is>
       </c>
       <c r="J25" t="n">
-        <v>9066046</v>
+        <v>1255671</v>
       </c>
       <c r="K25" t="inlineStr">
         <is>
@@ -1983,7 +1983,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>View all 3,143 employees</t>
+          <t>Discover all 3,145 employees</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -2012,7 +2012,7 @@
         </is>
       </c>
       <c r="J28" t="n">
-        <v>2238676</v>
+        <v>9277902</v>
       </c>
       <c r="K28" t="inlineStr">
         <is>
@@ -2067,7 +2067,7 @@
         </is>
       </c>
       <c r="J29" t="n">
-        <v>3872326</v>
+        <v>7681016</v>
       </c>
       <c r="K29" t="inlineStr">
         <is>
@@ -2122,7 +2122,7 @@
         </is>
       </c>
       <c r="J30" t="n">
-        <v>5343752</v>
+        <v>7450175</v>
       </c>
       <c r="K30" t="inlineStr">
         <is>
@@ -2148,7 +2148,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>View all 2,376 employees</t>
+          <t>Access all 2,378 employees</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -2177,7 +2177,7 @@
         </is>
       </c>
       <c r="J31" t="n">
-        <v>7702185</v>
+        <v>7225893</v>
       </c>
       <c r="K31" t="inlineStr">
         <is>
@@ -2203,7 +2203,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Discover all 1,911 employees</t>
+          <t>Access all 1,910 employees</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -2232,7 +2232,7 @@
         </is>
       </c>
       <c r="J32" t="n">
-        <v>4520192</v>
+        <v>5475998</v>
       </c>
       <c r="K32" t="inlineStr">
         <is>
@@ -2315,7 +2315,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>View all 722 employees</t>
+          <t>Discover all 722 employees</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -2344,7 +2344,7 @@
         </is>
       </c>
       <c r="J34" t="n">
-        <v>3377170</v>
+        <v>9700193</v>
       </c>
       <c r="K34" t="inlineStr">
         <is>
@@ -2370,7 +2370,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Access all 37 employees</t>
+          <t>View all 37 employees</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -2399,7 +2399,7 @@
         </is>
       </c>
       <c r="J35" t="n">
-        <v>1991014</v>
+        <v>6134151</v>
       </c>
       <c r="K35" t="inlineStr">
         <is>
@@ -2415,22 +2415,22 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Dallas, Texas</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Manufacturing</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Discover all 2,127 employees</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>1,001-5,000 employees</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -2440,12 +2440,12 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>https://www.interstatebatteries.com</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>interstatebatteries.com</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -2453,12 +2453,14 @@
           <t>https://www.linkedin.com/company/interstate-batteries</t>
         </is>
       </c>
-      <c r="J36" t="n">
-        <v>1233684</v>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>#1000</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -2480,7 +2482,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Access all 462 employees</t>
+          <t>View all 462 employees</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -2509,7 +2511,7 @@
         </is>
       </c>
       <c r="J37" t="n">
-        <v>7128960</v>
+        <v>2812787</v>
       </c>
       <c r="K37" t="inlineStr">
         <is>
@@ -2535,7 +2537,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>View all 1,916 employees</t>
+          <t>Discover all 1,885 employees</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -2564,7 +2566,7 @@
         </is>
       </c>
       <c r="J38" t="n">
-        <v>1118337</v>
+        <v>5943450</v>
       </c>
       <c r="K38" t="inlineStr">
         <is>
@@ -2637,22 +2639,22 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Houston, Texas</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Oil and Gas</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>View all 3,171 employees</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>1,001-5,000 employees</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -2662,12 +2664,12 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://www.mrcglobal.com</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>mrcglobal.com</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -2675,14 +2677,12 @@
           <t>https://www.linkedin.com/company/mrc-global</t>
         </is>
       </c>
-      <c r="J40" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="J40" t="n">
+        <v>1875436</v>
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Suite 2300</t>
         </is>
       </c>
     </row>
@@ -2847,7 +2847,7 @@
         </is>
       </c>
       <c r="J43" t="n">
-        <v>6718179</v>
+        <v>4342130</v>
       </c>
       <c r="K43" t="inlineStr">
         <is>
@@ -2920,22 +2920,22 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Houston, TX</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Packaging and Containers Manufacturing</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Discover all 1,324 employees</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>1,001-5,000 employees</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -2945,12 +2945,12 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>http://www.victorypackaging.com</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>victorypackaging.com</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
@@ -2958,14 +2958,12 @@
           <t>https://www.linkedin.com/company/victory-packaging</t>
         </is>
       </c>
-      <c r="J45" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="J45" t="n">
+        <v>3465758</v>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Ste. 1400</t>
         </is>
       </c>
     </row>
@@ -3044,7 +3042,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Discover all 408 employees</t>
+          <t>Discover all 411 employees</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -3073,7 +3071,7 @@
         </is>
       </c>
       <c r="J47" t="n">
-        <v>9149878</v>
+        <v>8669392</v>
       </c>
       <c r="K47" t="inlineStr">
         <is>
@@ -3099,7 +3097,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>View all 406 employees</t>
+          <t>Access all 406 employees</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -3128,7 +3126,7 @@
         </is>
       </c>
       <c r="J48" t="n">
-        <v>9915028</v>
+        <v>3709035</v>
       </c>
       <c r="K48" t="inlineStr">
         <is>
@@ -3211,7 +3209,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>View all 445 employees</t>
+          <t>Discover all 445 employees</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -3240,7 +3238,7 @@
         </is>
       </c>
       <c r="J50" t="n">
-        <v>5692170</v>
+        <v>5081958</v>
       </c>
       <c r="K50" t="inlineStr">
         <is>
@@ -3266,7 +3264,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>View all 1,898 employees</t>
+          <t>View all 1,899 employees</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -3295,7 +3293,7 @@
         </is>
       </c>
       <c r="J51" t="n">
-        <v>1547302</v>
+        <v>1283805</v>
       </c>
       <c r="K51" t="inlineStr">
         <is>
@@ -3321,7 +3319,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Discover all 162 employees</t>
+          <t>Access all 162 employees</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
@@ -3350,7 +3348,7 @@
         </is>
       </c>
       <c r="J52" t="n">
-        <v>9432655</v>
+        <v>3823190</v>
       </c>
       <c r="K52" t="inlineStr">
         <is>
@@ -3376,7 +3374,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>View all 69 employees</t>
+          <t>Access all 69 employees</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -3405,7 +3403,7 @@
         </is>
       </c>
       <c r="J53" t="n">
-        <v>6123333</v>
+        <v>7977563</v>
       </c>
       <c r="K53" t="inlineStr">
         <is>
@@ -3431,7 +3429,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Access all 603 employees</t>
+          <t>View all 603 employees</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -3460,7 +3458,7 @@
         </is>
       </c>
       <c r="J54" t="n">
-        <v>9052719</v>
+        <v>2617057</v>
       </c>
       <c r="K54" t="inlineStr">
         <is>
@@ -3486,7 +3484,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Discover all 2,170 employees</t>
+          <t>View all 2,171 employees</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -3515,7 +3513,7 @@
         </is>
       </c>
       <c r="J55" t="n">
-        <v>4438913</v>
+        <v>2097957</v>
       </c>
       <c r="K55" t="inlineStr">
         <is>
@@ -3655,7 +3653,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Access all 983 employees</t>
+          <t>View all 982 employees</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -3684,7 +3682,7 @@
         </is>
       </c>
       <c r="J58" t="n">
-        <v>3971142</v>
+        <v>1400464</v>
       </c>
       <c r="K58" t="inlineStr">
         <is>
@@ -3767,7 +3765,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Discover all 5,925 employees</t>
+          <t>View all 5,924 employees</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -3796,7 +3794,7 @@
         </is>
       </c>
       <c r="J60" t="n">
-        <v>8430095</v>
+        <v>3464691</v>
       </c>
       <c r="K60" t="inlineStr">
         <is>
@@ -3926,22 +3924,22 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Houston, TX</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Oil and Gas</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>View all 4,938 employees</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>1,001-5,000 employees</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -3951,12 +3949,12 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>http://www.citgo.com</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>citgo.com</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="I63" t="inlineStr">
@@ -3964,12 +3962,14 @@
           <t>https://www.linkedin.com/company/citgo-petroleum</t>
         </is>
       </c>
-      <c r="J63" t="n">
-        <v>9019552</v>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
       </c>
       <c r="K63" t="inlineStr">
         <is>
-          <t>Houston, TX 77077, US</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -4077,7 +4077,7 @@
         </is>
       </c>
       <c r="J65" t="n">
-        <v>9248294</v>
+        <v>2027737</v>
       </c>
       <c r="K65" t="inlineStr">
         <is>
@@ -4132,7 +4132,7 @@
         </is>
       </c>
       <c r="J66" t="n">
-        <v>7968464</v>
+        <v>9441682</v>
       </c>
       <c r="K66" t="inlineStr">
         <is>
@@ -4319,22 +4319,22 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Dallas, TX</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Wholesale Building Materials</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Discover all 1,836 employees</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>5,001-10,000 employees</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -4344,12 +4344,12 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>http://www.obe.com/</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>obe.com/</t>
         </is>
       </c>
       <c r="I70" t="inlineStr">
@@ -4357,14 +4357,12 @@
           <t>https://www.linkedin.com/company/oldcastle-buildingenvelope</t>
         </is>
       </c>
-      <c r="J70" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="J70" t="n">
+        <v>3341381</v>
       </c>
       <c r="K70" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Suite 1050</t>
         </is>
       </c>
     </row>
@@ -4386,7 +4384,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>View all 3,694 employees</t>
+          <t>View all 3,695 employees</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
@@ -4415,7 +4413,7 @@
         </is>
       </c>
       <c r="J71" t="n">
-        <v>8010350</v>
+        <v>8050882</v>
       </c>
       <c r="K71" t="inlineStr">
         <is>

</xml_diff>